<commit_message>
Renamed FilterBean values to data
</commit_message>
<xml_diff>
--- a/eca-report/src/main/resources/templates/experiments-report-template.xlsx
+++ b/eca-report/src/main/resources/templates/experiments-report-template.xlsx
@@ -55,8 +55,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
+            <charset val="1"/>
           </rPr>
           <t>Roman93:</t>
         </r>
@@ -65,8 +64,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 jx:if(condition="not empty(report.searchQuery)", lastCell="M3", areas=["A3:B3"])</t>
@@ -213,9 +211,6 @@
     <t>${filter.description}</t>
   </si>
   <si>
-    <t>${filter.values}</t>
-  </si>
-  <si>
     <t>Страница ${report.page} из ${report.totalPages}</t>
   </si>
   <si>
@@ -226,13 +221,16 @@
   </si>
   <si>
     <t>${report.searchQuery}</t>
+  </si>
+  <si>
+    <t>${filter.data}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,8 +279,21 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,13 +302,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.24994659260841701"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -360,22 +377,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -672,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -694,173 +713,188 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.6">
-      <c r="A1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
+      <c r="A1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
     </row>
     <row r="2" spans="1:13" ht="15.6">
-      <c r="A2" s="3"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
+      <c r="B4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="12"/>
+      <c r="A8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="13"/>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="1"/>

</xml_diff>

<commit_message>
Refactoring filter value string mapping
</commit_message>
<xml_diff>
--- a/eca-report/src/main/resources/templates/experiments-report-template.xlsx
+++ b/eca-report/src/main/resources/templates/experiments-report-template.xlsx
@@ -223,7 +223,7 @@
     <t>${report.searchQuery}</t>
   </si>
   <si>
-    <t>${filter.data}</t>
+    <t>${filter.filterData}</t>
   </si>
 </sst>
 </file>
@@ -393,15 +393,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -699,7 +699,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -708,8 +708,8 @@
     <col min="2" max="2" width="40.21875" customWidth="1"/>
     <col min="3" max="3" width="28.88671875" customWidth="1"/>
     <col min="4" max="4" width="36.5546875" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
     <col min="7" max="7" width="51.88671875" customWidth="1"/>
     <col min="8" max="8" width="49.77734375" customWidth="1"/>
     <col min="9" max="9" width="27" customWidth="1"/>
@@ -720,24 +720,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.6">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
     </row>
     <row r="2" spans="1:13" ht="15.6">
-      <c r="A2" s="11"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -752,42 +752,42 @@
       <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="2"/>
@@ -887,21 +887,21 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="9"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="14"/>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="1"/>

</xml_diff>

<commit_message>
Changes in experiment-report template
</commit_message>
<xml_diff>
--- a/eca-report/src/main/resources/templates/experiments-report-template.xlsx
+++ b/eca-report/src/main/resources/templates/experiments-report-template.xlsx
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -711,7 +711,7 @@
     <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
     <col min="7" max="7" width="51.88671875" customWidth="1"/>
-    <col min="8" max="8" width="49.77734375" customWidth="1"/>
+    <col min="8" max="8" width="57.77734375" customWidth="1"/>
     <col min="9" max="9" width="27" customWidth="1"/>
     <col min="10" max="10" width="30.88671875" customWidth="1"/>
     <col min="11" max="11" width="34.33203125" customWidth="1"/>

</xml_diff>

<commit_message>
Added evaluation-logs report template
</commit_message>
<xml_diff>
--- a/eca-report/src/main/resources/templates/experiments-report-template.xlsx
+++ b/eca-report/src/main/resources/templates/experiments-report-template.xlsx
@@ -387,21 +387,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -698,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -720,74 +728,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="15.6">
-      <c r="A2" s="7"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="2"/>
@@ -805,103 +813,103 @@
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="14"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="11"/>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="1"/>

</xml_diff>

<commit_message>
#ES-159 - updated experiments-report-template.xlsx
</commit_message>
<xml_diff>
--- a/eca-report/src/main/resources/templates/experiments-report-template.xlsx
+++ b/eca-report/src/main/resources/templates/experiments-report-template.xlsx
@@ -46,7 +46,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="N8")</t>
+jx:area(lastCell="M8")</t>
         </r>
       </text>
     </comment>
@@ -70,7 +70,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:if(condition="not empty(report.searchQuery)", lastCell="N3", areas=["A3:B3"])</t>
+jx:if(condition="not empty(report.searchQuery)", lastCell="M3", areas=["A3:B3"])</t>
         </r>
       </text>
     </comment>
@@ -94,7 +94,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="report.filters" var="filter" lastCell="N4")</t>
+jx:each(items="report.filters" var="filter" lastCell="M4")</t>
         </r>
       </text>
     </comment>
@@ -118,7 +118,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="report.items" var="experiment" lastCell="N7")</t>
+jx:each(items="report.items" var="experiment" lastCell="M7")</t>
         </r>
       </text>
     </comment>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Отчет по заявкам на эксперимент</t>
   </si>
@@ -180,9 +180,6 @@
     <t>Дата окончания эксперимента</t>
   </si>
   <si>
-    <t>Дата отправки результатов</t>
-  </si>
-  <si>
     <t>Дата удаления результатов</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
   </si>
   <si>
     <t>${experiment.endDate}</t>
-  </si>
-  <si>
-    <t>${experiment.sentDate}</t>
   </si>
   <si>
     <t>${experiment.deletedDate}</t>
@@ -354,11 +348,6 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -378,6 +367,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -740,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -760,213 +754,200 @@
     <col min="10" max="10" width="27" customWidth="1"/>
     <col min="11" max="11" width="30.88671875" customWidth="1"/>
     <col min="12" max="12" width="34.33203125" customWidth="1"/>
-    <col min="13" max="13" width="31.44140625" customWidth="1"/>
-    <col min="14" max="14" width="31.5546875" customWidth="1"/>
-    <col min="15" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="13" max="13" width="31.5546875" customWidth="1"/>
+    <col min="14" max="1024" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.6">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" ht="15.6">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
     </row>
-    <row r="2" spans="1:14" ht="15.6">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
+    <row r="2" spans="1:13" ht="15.6">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="14.85" customHeight="1">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:13" ht="14.85" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
     </row>
-    <row r="4" spans="1:14" ht="14.85" customHeight="1">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:13" ht="14.85" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
+    <row r="5" spans="1:13">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:13">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="M6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="9" t="s">
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="B7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="M7" s="11" t="s">
+    <row r="8" spans="1:13">
+      <c r="A8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="N7" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="B4:N4"/>
-    <mergeCell ref="A8:N8"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="A8:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
#ES-213 - updated experiments-report-template.xlsx
</commit_message>
<xml_diff>
--- a/eca-report/src/main/resources/templates/experiments-report-template.xlsx
+++ b/eca-report/src/main/resources/templates/experiments-report-template.xlsx
@@ -201,12 +201,6 @@
     <t>${experiment.email}</t>
   </si>
   <si>
-    <t>${experiment.trainingDataAbsolutePath}</t>
-  </si>
-  <si>
-    <t>${experiment.experimentAbsolutePath}</t>
-  </si>
-  <si>
     <t>${experiment.evaluationTotalTime}</t>
   </si>
   <si>
@@ -223,6 +217,12 @@
   </si>
   <si>
     <t>Страница ${report.page} из ${report.totalPages}</t>
+  </si>
+  <si>
+    <t>${experiment.relationName}</t>
+  </si>
+  <si>
+    <t>${experiment.experimentPath}</t>
   </si>
 </sst>
 </file>
@@ -346,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -372,6 +372,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -736,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -903,31 +906,31 @@
       <c r="F7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="J7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="K7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="L7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="M7" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>

</xml_diff>

<commit_message>
#ES-244 - updated experiments-report-template.xlsx
</commit_message>
<xml_diff>
--- a/eca-report/src/main/resources/templates/experiments-report-template.xlsx
+++ b/eca-report/src/main/resources/templates/experiments-report-template.xlsx
@@ -46,7 +46,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="M8")</t>
+jx:area(lastCell="L8")</t>
         </r>
       </text>
     </comment>
@@ -70,7 +70,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:if(condition="not empty(report.searchQuery)", lastCell="M3", areas=["A3:B3"])</t>
+jx:if(condition="not empty(report.searchQuery)", lastCell="L3", areas=["A3:B3"])</t>
         </r>
       </text>
     </comment>
@@ -94,7 +94,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="report.filters" var="filter" lastCell="M4")</t>
+jx:each(items="report.filters" var="filter" lastCell="L4")</t>
         </r>
       </text>
     </comment>
@@ -118,7 +118,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="report.items" var="experiment" lastCell="M7")</t>
+jx:each(items="report.items" var="experiment" lastCell="L7")</t>
         </r>
       </text>
     </comment>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Отчет по заявкам на эксперимент</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Метод оценки точности</t>
   </si>
   <si>
-    <t>Имя заявки</t>
-  </si>
-  <si>
     <t>Email заявки</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
   </si>
   <si>
     <t>${experiment.evaluationMethod}</t>
-  </si>
-  <si>
-    <t>${experiment.firstName}</t>
   </si>
   <si>
     <t>${experiment.email}</t>
@@ -367,14 +361,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -737,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -749,36 +743,34 @@
     <col min="2" max="2" width="40.21875" customWidth="1"/>
     <col min="3" max="3" width="28.88671875" customWidth="1"/>
     <col min="4" max="4" width="36.5546875" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="51.88671875" customWidth="1"/>
-    <col min="8" max="8" width="59.5546875" customWidth="1"/>
-    <col min="9" max="9" width="37.88671875" customWidth="1"/>
-    <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="11" width="30.88671875" customWidth="1"/>
-    <col min="12" max="12" width="34.33203125" customWidth="1"/>
-    <col min="13" max="13" width="31.5546875" customWidth="1"/>
-    <col min="14" max="1024" width="8.5546875" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="6" max="6" width="51.88671875" customWidth="1"/>
+    <col min="7" max="7" width="59.5546875" customWidth="1"/>
+    <col min="8" max="8" width="37.88671875" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
+    <col min="10" max="10" width="30.88671875" customWidth="1"/>
+    <col min="11" max="11" width="34.33203125" customWidth="1"/>
+    <col min="12" max="12" width="31.5546875" customWidth="1"/>
+    <col min="13" max="1023" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.6">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:12" ht="15.6">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
-    <row r="2" spans="1:13" ht="15.6">
+    <row r="2" spans="1:12" ht="15.6">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -791,47 +783,44 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" ht="14.85" customHeight="1">
+    <row r="3" spans="1:12" ht="14.85" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:13" ht="14.85" customHeight="1">
+    <row r="4" spans="1:12" ht="14.85" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:12">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -844,9 +833,8 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:12">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
@@ -883,74 +871,67 @@
       <c r="L6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="6" t="s">
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="B7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="8" t="s">
+    <row r="8" spans="1:12">
+      <c r="A8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="A8:M8"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="A8:L8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>